<commit_message>
Add state_vehicle and euro in fleet.vehicle - fix 5
</commit_message>
<xml_diff>
--- a/dipendenti/file.xlsx
+++ b/dipendenti/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/Desktop/FUTURA/Dev/ODOOSH/TEST-import-anomalie/futura/dipendenti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DEFA2-5B8E-E947-BBE0-44CC51E966ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C6978-8293-A645-83CE-DB8ACEE14EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15680" xr2:uid="{9AE6A15F-E659-554F-9F01-889FED0F391C}"/>
   </bookViews>
@@ -1378,10 +1378,13 @@
   <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:B281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>